<commit_message>
lesson 1: complete dogs breeds competition
</commit_message>
<xml_diff>
--- a/competitions.xlsx
+++ b/competitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Competition Name</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/c/dog-breed-identification</t>
+  </si>
+  <si>
+    <t>Dog Breeds</t>
   </si>
 </sst>
 </file>
@@ -79,8 +85,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -127,15 +133,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -144,7 +149,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,55 +430,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="11" max="11" width="30" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
+    <col min="11" max="11" width="27.5" customWidth="1"/>
     <col min="12" max="12" width="55.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -481,23 +486,23 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>I2/J2</f>
         <v>7.3059360730593603E-2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>43196</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H2">
@@ -511,6 +516,42 @@
       </c>
       <c r="L2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2">
+        <f>I3/J3</f>
+        <v>0.24183514774494558</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43201</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>0.21451000000000001</v>
+      </c>
+      <c r="I3">
+        <v>311</v>
+      </c>
+      <c r="J3">
+        <v>1286</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>